<commit_message>
add jenkins trouble shooting
</commit_message>
<xml_diff>
--- a/certificate/sc-japan/수험서주제정리.xlsx
+++ b/certificate/sc-japan/수험서주제정리.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="618">
   <si>
     <t>장</t>
     <phoneticPr fontId="2"/>
@@ -13297,6 +13297,317 @@
         <scheme val="minor"/>
       </rPr>
       <t>법제도</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>단계</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>단계</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>단계</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>형광펜</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>단계</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>진행중</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>배경색</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>분홍</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>노랑</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>파랑</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>키워드, 중요 내용</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>장,절,주제 (대/중/소 제목) 정리</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>레벨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>레벨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>제목</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>정리</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 66</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>절</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 217</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>주제</t>
     </r>
     <phoneticPr fontId="2"/>
   </si>
@@ -13308,7 +13619,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;/&quot;d;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13376,8 +13687,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13399,6 +13725,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -13426,7 +13770,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -13511,16 +13855,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13531,6 +13905,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFF66FF"/>
       <color rgb="FFE8B9FF"/>
       <color rgb="FFCC66FF"/>
     </mruColors>
@@ -13812,8 +14188,8 @@
   <dimension ref="A1:K219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E175" sqref="E175"/>
+      <pane ySplit="2" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -16099,7 +16475,7 @@
       <c r="I77" s="19">
         <v>43142</v>
       </c>
-      <c r="J77" s="30">
+      <c r="J77" s="28">
         <v>223</v>
       </c>
     </row>
@@ -16131,7 +16507,7 @@
       <c r="I78" s="19">
         <v>43142</v>
       </c>
-      <c r="J78" s="30"/>
+      <c r="J78" s="28"/>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="12">
@@ -17251,1210 +17627,1210 @@
       <c r="J115" s="27"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="20">
+      <c r="A116" s="27">
         <v>114</v>
       </c>
-      <c r="B116" s="20">
+      <c r="B116" s="27">
         <v>5</v>
       </c>
-      <c r="C116" s="21" t="s">
+      <c r="C116" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D116" s="22">
+      <c r="D116" s="24">
         <v>5.6</v>
       </c>
-      <c r="E116" s="21" t="s">
+      <c r="E116" s="25" t="s">
         <v>578</v>
       </c>
-      <c r="F116" s="22" t="s">
+      <c r="F116" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="G116" s="21" t="s">
+      <c r="G116" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="H116" s="22"/>
-      <c r="I116" s="23"/>
-      <c r="J116" s="20">
+      <c r="H116" s="24"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="27">
         <v>371</v>
       </c>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="20">
+      <c r="A117" s="27">
         <v>115</v>
       </c>
-      <c r="B117" s="20">
+      <c r="B117" s="27">
         <v>5</v>
       </c>
-      <c r="C117" s="21" t="s">
+      <c r="C117" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D117" s="22">
+      <c r="D117" s="24">
         <v>5.6</v>
       </c>
-      <c r="E117" s="21" t="s">
+      <c r="E117" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F117" s="22" t="s">
+      <c r="F117" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="G117" s="21" t="s">
+      <c r="G117" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="H117" s="22"/>
-      <c r="I117" s="23"/>
-      <c r="J117" s="20"/>
+      <c r="H117" s="24"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="27"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="20">
+      <c r="A118" s="27">
         <v>116</v>
       </c>
-      <c r="B118" s="20">
+      <c r="B118" s="27">
         <v>5</v>
       </c>
-      <c r="C118" s="21" t="s">
+      <c r="C118" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D118" s="22">
+      <c r="D118" s="24">
         <v>5.6</v>
       </c>
-      <c r="E118" s="21" t="s">
+      <c r="E118" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F118" s="22" t="s">
+      <c r="F118" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="G118" s="21" t="s">
+      <c r="G118" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="H118" s="22"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="20">
+      <c r="H118" s="24"/>
+      <c r="I118" s="26"/>
+      <c r="J118" s="27">
         <v>383</v>
       </c>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="20">
+      <c r="A119" s="27">
         <v>117</v>
       </c>
-      <c r="B119" s="20">
+      <c r="B119" s="27">
         <v>5</v>
       </c>
-      <c r="C119" s="21" t="s">
+      <c r="C119" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D119" s="22">
+      <c r="D119" s="24">
         <v>5.6</v>
       </c>
-      <c r="E119" s="21" t="s">
+      <c r="E119" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F119" s="22" t="s">
+      <c r="F119" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="G119" s="21" t="s">
+      <c r="G119" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="H119" s="22"/>
-      <c r="I119" s="23"/>
-      <c r="J119" s="20"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="26"/>
+      <c r="J119" s="27"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="20">
+      <c r="A120" s="27">
         <v>118</v>
       </c>
-      <c r="B120" s="20">
+      <c r="B120" s="27">
         <v>5</v>
       </c>
-      <c r="C120" s="21" t="s">
+      <c r="C120" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D120" s="22">
+      <c r="D120" s="24">
         <v>5.6</v>
       </c>
-      <c r="E120" s="21" t="s">
+      <c r="E120" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F120" s="22" t="s">
+      <c r="F120" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="G120" s="21" t="s">
+      <c r="G120" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="H120" s="22"/>
-      <c r="I120" s="23"/>
-      <c r="J120" s="20"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="26"/>
+      <c r="J120" s="27"/>
     </row>
     <row r="121" spans="1:10">
-      <c r="A121" s="20">
+      <c r="A121" s="27">
         <v>119</v>
       </c>
-      <c r="B121" s="20">
+      <c r="B121" s="27">
         <v>5</v>
       </c>
-      <c r="C121" s="21" t="s">
+      <c r="C121" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D121" s="22">
+      <c r="D121" s="24">
         <v>5.6</v>
       </c>
-      <c r="E121" s="21" t="s">
+      <c r="E121" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F121" s="22" t="s">
+      <c r="F121" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="G121" s="21" t="s">
+      <c r="G121" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="H121" s="22"/>
-      <c r="I121" s="23"/>
-      <c r="J121" s="20"/>
+      <c r="H121" s="24"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="27"/>
     </row>
     <row r="122" spans="1:10">
-      <c r="A122" s="20">
+      <c r="A122" s="27">
         <v>120</v>
       </c>
-      <c r="B122" s="20">
+      <c r="B122" s="27">
         <v>5</v>
       </c>
-      <c r="C122" s="21" t="s">
+      <c r="C122" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D122" s="22" t="s">
+      <c r="D122" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="E122" s="21" t="s">
+      <c r="E122" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F122" s="22" t="s">
+      <c r="F122" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="G122" s="21" t="s">
+      <c r="G122" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="H122" s="22"/>
-      <c r="I122" s="23"/>
-      <c r="J122" s="20"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="27"/>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="20">
+      <c r="A123" s="27">
         <v>121</v>
       </c>
-      <c r="B123" s="20">
+      <c r="B123" s="27">
         <v>5</v>
       </c>
-      <c r="C123" s="21" t="s">
+      <c r="C123" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D123" s="22" t="s">
+      <c r="D123" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="E123" s="21" t="s">
+      <c r="E123" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F123" s="22" t="s">
+      <c r="F123" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="G123" s="21" t="s">
+      <c r="G123" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="H123" s="22"/>
-      <c r="I123" s="23"/>
-      <c r="J123" s="20"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="26"/>
+      <c r="J123" s="27"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="20">
+      <c r="A124" s="27">
         <v>122</v>
       </c>
-      <c r="B124" s="20">
+      <c r="B124" s="27">
         <v>5</v>
       </c>
-      <c r="C124" s="21" t="s">
+      <c r="C124" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D124" s="22" t="s">
+      <c r="D124" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="E124" s="21" t="s">
+      <c r="E124" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F124" s="22" t="s">
+      <c r="F124" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="G124" s="21" t="s">
+      <c r="G124" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="H124" s="22"/>
-      <c r="I124" s="23"/>
-      <c r="J124" s="20"/>
+      <c r="H124" s="24"/>
+      <c r="I124" s="26"/>
+      <c r="J124" s="27"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="20">
+      <c r="A125" s="27">
         <v>123</v>
       </c>
-      <c r="B125" s="20">
+      <c r="B125" s="27">
         <v>5</v>
       </c>
-      <c r="C125" s="21" t="s">
+      <c r="C125" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D125" s="22">
+      <c r="D125" s="24">
         <v>5.7</v>
       </c>
-      <c r="E125" s="21" t="s">
+      <c r="E125" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="F125" s="22" t="s">
+      <c r="F125" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="G125" s="20" t="s">
+      <c r="G125" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="H125" s="22"/>
-      <c r="I125" s="23"/>
-      <c r="J125" s="20"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="26"/>
+      <c r="J125" s="27"/>
     </row>
     <row r="126" spans="1:10">
-      <c r="A126" s="20">
+      <c r="A126" s="27">
         <v>124</v>
       </c>
-      <c r="B126" s="20">
+      <c r="B126" s="27">
         <v>5</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C126" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D126" s="22" t="s">
+      <c r="D126" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E126" s="21" t="s">
+      <c r="E126" s="25" t="s">
         <v>579</v>
       </c>
-      <c r="F126" s="22" t="s">
+      <c r="F126" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="G126" s="21" t="s">
+      <c r="G126" s="25" t="s">
         <v>580</v>
       </c>
-      <c r="H126" s="22"/>
-      <c r="I126" s="23"/>
-      <c r="J126" s="20"/>
+      <c r="H126" s="24"/>
+      <c r="I126" s="26"/>
+      <c r="J126" s="27"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="20">
+      <c r="A127" s="27">
         <v>125</v>
       </c>
-      <c r="B127" s="20">
+      <c r="B127" s="27">
         <v>5</v>
       </c>
-      <c r="C127" s="21" t="s">
+      <c r="C127" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D127" s="22" t="s">
+      <c r="D127" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="E127" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F127" s="22" t="s">
+      <c r="F127" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="G127" s="21" t="s">
+      <c r="G127" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="H127" s="22"/>
-      <c r="I127" s="23"/>
-      <c r="J127" s="20"/>
+      <c r="H127" s="24"/>
+      <c r="I127" s="26"/>
+      <c r="J127" s="27"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="20">
+      <c r="A128" s="27">
         <v>126</v>
       </c>
-      <c r="B128" s="20">
+      <c r="B128" s="27">
         <v>5</v>
       </c>
-      <c r="C128" s="21" t="s">
+      <c r="C128" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D128" s="22" t="s">
+      <c r="D128" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E128" s="21" t="s">
+      <c r="E128" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F128" s="22" t="s">
+      <c r="F128" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="G128" s="21" t="s">
+      <c r="G128" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="H128" s="22"/>
-      <c r="I128" s="23"/>
-      <c r="J128" s="20"/>
+      <c r="H128" s="24"/>
+      <c r="I128" s="26"/>
+      <c r="J128" s="27"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="20">
+      <c r="A129" s="27">
         <v>127</v>
       </c>
-      <c r="B129" s="20">
+      <c r="B129" s="27">
         <v>5</v>
       </c>
-      <c r="C129" s="21" t="s">
+      <c r="C129" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D129" s="22" t="s">
+      <c r="D129" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E129" s="21" t="s">
+      <c r="E129" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F129" s="22" t="s">
+      <c r="F129" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="G129" s="21" t="s">
+      <c r="G129" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="H129" s="22"/>
-      <c r="I129" s="23"/>
-      <c r="J129" s="20"/>
+      <c r="H129" s="24"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="27"/>
     </row>
     <row r="130" spans="1:10">
-      <c r="A130" s="20">
+      <c r="A130" s="27">
         <v>128</v>
       </c>
-      <c r="B130" s="20">
+      <c r="B130" s="27">
         <v>5</v>
       </c>
-      <c r="C130" s="21" t="s">
+      <c r="C130" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D130" s="20">
+      <c r="D130" s="27">
         <v>5.9</v>
       </c>
-      <c r="E130" s="21" t="s">
+      <c r="E130" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="F130" s="22" t="s">
+      <c r="F130" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="G130" s="21" t="s">
+      <c r="G130" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="H130" s="22"/>
-      <c r="I130" s="23"/>
-      <c r="J130" s="20"/>
+      <c r="H130" s="24"/>
+      <c r="I130" s="26"/>
+      <c r="J130" s="27"/>
     </row>
     <row r="131" spans="1:10">
-      <c r="A131" s="20">
+      <c r="A131" s="27">
         <v>129</v>
       </c>
-      <c r="B131" s="20">
+      <c r="B131" s="27">
         <v>5</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C131" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D131" s="20">
+      <c r="D131" s="27">
         <v>5.9</v>
       </c>
-      <c r="E131" s="21" t="s">
+      <c r="E131" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="F131" s="22" t="s">
+      <c r="F131" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="G131" s="21" t="s">
+      <c r="G131" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="H131" s="22"/>
-      <c r="I131" s="23"/>
-      <c r="J131" s="20"/>
+      <c r="H131" s="24"/>
+      <c r="I131" s="26"/>
+      <c r="J131" s="27"/>
     </row>
     <row r="132" spans="1:10">
-      <c r="A132" s="20">
+      <c r="A132" s="27">
         <v>130</v>
       </c>
-      <c r="B132" s="20">
+      <c r="B132" s="27">
         <v>5</v>
       </c>
-      <c r="C132" s="21" t="s">
+      <c r="C132" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D132" s="20">
+      <c r="D132" s="27">
         <v>5.9</v>
       </c>
-      <c r="E132" s="21" t="s">
+      <c r="E132" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="F132" s="22" t="s">
+      <c r="F132" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="G132" s="21" t="s">
+      <c r="G132" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="H132" s="22"/>
-      <c r="I132" s="23"/>
-      <c r="J132" s="20"/>
+      <c r="H132" s="24"/>
+      <c r="I132" s="26"/>
+      <c r="J132" s="27"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="20">
+      <c r="A133" s="27">
         <v>131</v>
       </c>
-      <c r="B133" s="20">
+      <c r="B133" s="27">
         <v>6</v>
       </c>
-      <c r="C133" s="21" t="s">
+      <c r="C133" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D133" s="22">
+      <c r="D133" s="24">
         <v>6.1</v>
       </c>
-      <c r="E133" s="21" t="s">
+      <c r="E133" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F133" s="22" t="s">
+      <c r="F133" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="G133" s="21" t="s">
+      <c r="G133" s="25" t="s">
         <v>329</v>
       </c>
-      <c r="H133" s="22"/>
-      <c r="I133" s="23"/>
-      <c r="J133" s="20">
+      <c r="H133" s="24"/>
+      <c r="I133" s="26"/>
+      <c r="J133" s="27">
         <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="20">
+      <c r="A134" s="27">
         <v>132</v>
       </c>
-      <c r="B134" s="20">
+      <c r="B134" s="27">
         <v>6</v>
       </c>
-      <c r="C134" s="21" t="s">
+      <c r="C134" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D134" s="22">
+      <c r="D134" s="24">
         <v>6.1</v>
       </c>
-      <c r="E134" s="21" t="s">
+      <c r="E134" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F134" s="22" t="s">
+      <c r="F134" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="G134" s="21" t="s">
+      <c r="G134" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="H134" s="22"/>
-      <c r="I134" s="23"/>
-      <c r="J134" s="20"/>
+      <c r="H134" s="24"/>
+      <c r="I134" s="26"/>
+      <c r="J134" s="27"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="20">
+      <c r="A135" s="27">
         <v>133</v>
       </c>
-      <c r="B135" s="20">
+      <c r="B135" s="27">
         <v>6</v>
       </c>
-      <c r="C135" s="21" t="s">
+      <c r="C135" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D135" s="22" t="s">
+      <c r="D135" s="24" t="s">
         <v>528</v>
       </c>
-      <c r="E135" s="21" t="s">
+      <c r="E135" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="F135" s="22" t="s">
+      <c r="F135" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="G135" s="21" t="s">
+      <c r="G135" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="H135" s="22"/>
-      <c r="I135" s="23"/>
-      <c r="J135" s="20">
+      <c r="H135" s="24"/>
+      <c r="I135" s="26"/>
+      <c r="J135" s="27">
         <v>428</v>
       </c>
     </row>
     <row r="136" spans="1:10">
-      <c r="A136" s="20">
+      <c r="A136" s="27">
         <v>134</v>
       </c>
-      <c r="B136" s="20">
+      <c r="B136" s="27">
         <v>6</v>
       </c>
-      <c r="C136" s="21" t="s">
+      <c r="C136" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D136" s="22" t="s">
+      <c r="D136" s="24" t="s">
         <v>528</v>
       </c>
-      <c r="E136" s="21" t="s">
+      <c r="E136" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="F136" s="22" t="s">
+      <c r="F136" s="24" t="s">
         <v>334</v>
       </c>
-      <c r="G136" s="21" t="s">
+      <c r="G136" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="H136" s="22"/>
-      <c r="I136" s="23"/>
-      <c r="J136" s="20"/>
+      <c r="H136" s="24"/>
+      <c r="I136" s="26"/>
+      <c r="J136" s="27"/>
     </row>
     <row r="137" spans="1:10">
-      <c r="A137" s="20">
+      <c r="A137" s="27">
         <v>135</v>
       </c>
-      <c r="B137" s="20">
+      <c r="B137" s="27">
         <v>6</v>
       </c>
-      <c r="C137" s="21" t="s">
+      <c r="C137" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D137" s="22">
+      <c r="D137" s="24">
         <v>6.3</v>
       </c>
-      <c r="E137" s="21" t="s">
+      <c r="E137" s="25" t="s">
         <v>581</v>
       </c>
-      <c r="F137" s="22" t="s">
+      <c r="F137" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="G137" s="21" t="s">
+      <c r="G137" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="H137" s="22"/>
-      <c r="I137" s="23"/>
-      <c r="J137" s="20"/>
+      <c r="H137" s="24"/>
+      <c r="I137" s="26"/>
+      <c r="J137" s="27"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="20">
+      <c r="A138" s="27">
         <v>136</v>
       </c>
-      <c r="B138" s="20">
+      <c r="B138" s="27">
         <v>6</v>
       </c>
-      <c r="C138" s="21" t="s">
+      <c r="C138" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D138" s="22">
+      <c r="D138" s="24">
         <v>6.4</v>
       </c>
-      <c r="E138" s="21" t="s">
+      <c r="E138" s="25" t="s">
         <v>582</v>
       </c>
-      <c r="F138" s="22" t="s">
+      <c r="F138" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="G138" s="21" t="s">
+      <c r="G138" s="25" t="s">
         <v>339</v>
       </c>
-      <c r="H138" s="22"/>
-      <c r="I138" s="23"/>
-      <c r="J138" s="20"/>
+      <c r="H138" s="24"/>
+      <c r="I138" s="26"/>
+      <c r="J138" s="27"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="20">
+      <c r="A139" s="27">
         <v>137</v>
       </c>
-      <c r="B139" s="20">
+      <c r="B139" s="27">
         <v>6</v>
       </c>
-      <c r="C139" s="21" t="s">
+      <c r="C139" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D139" s="22">
+      <c r="D139" s="24">
         <v>6.4</v>
       </c>
-      <c r="E139" s="21" t="s">
+      <c r="E139" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F139" s="22" t="s">
+      <c r="F139" s="24" t="s">
         <v>340</v>
       </c>
-      <c r="G139" s="21" t="s">
+      <c r="G139" s="25" t="s">
         <v>341</v>
       </c>
-      <c r="H139" s="22"/>
-      <c r="I139" s="23"/>
-      <c r="J139" s="20"/>
+      <c r="H139" s="24"/>
+      <c r="I139" s="26"/>
+      <c r="J139" s="27"/>
     </row>
     <row r="140" spans="1:10">
-      <c r="A140" s="20">
+      <c r="A140" s="27">
         <v>138</v>
       </c>
-      <c r="B140" s="20">
+      <c r="B140" s="27">
         <v>6</v>
       </c>
-      <c r="C140" s="21" t="s">
+      <c r="C140" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D140" s="22">
+      <c r="D140" s="24">
         <v>6.4</v>
       </c>
-      <c r="E140" s="21" t="s">
+      <c r="E140" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F140" s="22" t="s">
+      <c r="F140" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="G140" s="21" t="s">
+      <c r="G140" s="25" t="s">
         <v>343</v>
       </c>
-      <c r="H140" s="22"/>
-      <c r="I140" s="23"/>
-      <c r="J140" s="20"/>
+      <c r="H140" s="24"/>
+      <c r="I140" s="26"/>
+      <c r="J140" s="27"/>
     </row>
     <row r="141" spans="1:10">
-      <c r="A141" s="20">
+      <c r="A141" s="27">
         <v>139</v>
       </c>
-      <c r="B141" s="20">
+      <c r="B141" s="27">
         <v>6</v>
       </c>
-      <c r="C141" s="21" t="s">
+      <c r="C141" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D141" s="22">
+      <c r="D141" s="24">
         <v>6.5</v>
       </c>
-      <c r="E141" s="21" t="s">
+      <c r="E141" s="25" t="s">
         <v>583</v>
       </c>
-      <c r="F141" s="22" t="s">
+      <c r="F141" s="24" t="s">
         <v>344</v>
       </c>
-      <c r="G141" s="21" t="s">
+      <c r="G141" s="25" t="s">
         <v>345</v>
       </c>
-      <c r="H141" s="22"/>
-      <c r="I141" s="23"/>
-      <c r="J141" s="20"/>
+      <c r="H141" s="24"/>
+      <c r="I141" s="26"/>
+      <c r="J141" s="27"/>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142" s="20">
+      <c r="A142" s="27">
         <v>140</v>
       </c>
-      <c r="B142" s="20">
+      <c r="B142" s="27">
         <v>6</v>
       </c>
-      <c r="C142" s="21" t="s">
+      <c r="C142" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D142" s="22">
+      <c r="D142" s="24">
         <v>6.5</v>
       </c>
-      <c r="E142" s="21" t="s">
+      <c r="E142" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F142" s="22" t="s">
+      <c r="F142" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="G142" s="21" t="s">
+      <c r="G142" s="25" t="s">
         <v>347</v>
       </c>
-      <c r="H142" s="22"/>
-      <c r="I142" s="23"/>
-      <c r="J142" s="20"/>
+      <c r="H142" s="24"/>
+      <c r="I142" s="26"/>
+      <c r="J142" s="27"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="20">
+      <c r="A143" s="27">
         <v>141</v>
       </c>
-      <c r="B143" s="20">
+      <c r="B143" s="27">
         <v>6</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C143" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D143" s="22">
+      <c r="D143" s="24">
         <v>6.5</v>
       </c>
-      <c r="E143" s="21" t="s">
+      <c r="E143" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F143" s="22" t="s">
+      <c r="F143" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="G143" s="21" t="s">
+      <c r="G143" s="25" t="s">
         <v>349</v>
       </c>
-      <c r="H143" s="22"/>
-      <c r="I143" s="23"/>
-      <c r="J143" s="20"/>
+      <c r="H143" s="24"/>
+      <c r="I143" s="26"/>
+      <c r="J143" s="27"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="20">
+      <c r="A144" s="27">
         <v>142</v>
       </c>
-      <c r="B144" s="20">
+      <c r="B144" s="27">
         <v>6</v>
       </c>
-      <c r="C144" s="21" t="s">
+      <c r="C144" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D144" s="22">
+      <c r="D144" s="24">
         <v>6.6</v>
       </c>
-      <c r="E144" s="21" t="s">
+      <c r="E144" s="25" t="s">
         <v>584</v>
       </c>
-      <c r="F144" s="22" t="s">
+      <c r="F144" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="G144" s="21" t="s">
+      <c r="G144" s="25" t="s">
         <v>351</v>
       </c>
-      <c r="H144" s="22"/>
-      <c r="I144" s="23"/>
-      <c r="J144" s="20"/>
+      <c r="H144" s="24"/>
+      <c r="I144" s="26"/>
+      <c r="J144" s="27"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="20">
+      <c r="A145" s="27">
         <v>143</v>
       </c>
-      <c r="B145" s="20">
+      <c r="B145" s="27">
         <v>6</v>
       </c>
-      <c r="C145" s="21" t="s">
+      <c r="C145" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D145" s="22">
+      <c r="D145" s="24">
         <v>6.6</v>
       </c>
-      <c r="E145" s="21" t="s">
+      <c r="E145" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F145" s="22" t="s">
+      <c r="F145" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="G145" s="21" t="s">
+      <c r="G145" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="H145" s="22"/>
-      <c r="I145" s="23"/>
-      <c r="J145" s="20"/>
+      <c r="H145" s="24"/>
+      <c r="I145" s="26"/>
+      <c r="J145" s="27"/>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146" s="20">
+      <c r="A146" s="27">
         <v>144</v>
       </c>
-      <c r="B146" s="20">
+      <c r="B146" s="27">
         <v>6</v>
       </c>
-      <c r="C146" s="21" t="s">
+      <c r="C146" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D146" s="22">
+      <c r="D146" s="24">
         <v>6.7</v>
       </c>
-      <c r="E146" s="21" t="s">
+      <c r="E146" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F146" s="22" t="s">
+      <c r="F146" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="G146" s="21" t="s">
+      <c r="G146" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="H146" s="22"/>
-      <c r="I146" s="23"/>
-      <c r="J146" s="20"/>
+      <c r="H146" s="24"/>
+      <c r="I146" s="26"/>
+      <c r="J146" s="27"/>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147" s="20">
+      <c r="A147" s="27">
         <v>145</v>
       </c>
-      <c r="B147" s="20">
+      <c r="B147" s="27">
         <v>6</v>
       </c>
-      <c r="C147" s="21" t="s">
+      <c r="C147" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D147" s="22">
+      <c r="D147" s="24">
         <v>6.7</v>
       </c>
-      <c r="E147" s="21" t="s">
+      <c r="E147" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F147" s="22" t="s">
+      <c r="F147" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="G147" s="21" t="s">
+      <c r="G147" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="H147" s="22"/>
-      <c r="I147" s="23"/>
-      <c r="J147" s="20"/>
+      <c r="H147" s="24"/>
+      <c r="I147" s="26"/>
+      <c r="J147" s="27"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="20">
+      <c r="A148" s="27">
         <v>146</v>
       </c>
-      <c r="B148" s="20">
+      <c r="B148" s="27">
         <v>6</v>
       </c>
-      <c r="C148" s="21" t="s">
+      <c r="C148" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D148" s="22">
+      <c r="D148" s="24">
         <v>6.7</v>
       </c>
-      <c r="E148" s="21" t="s">
+      <c r="E148" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F148" s="22" t="s">
+      <c r="F148" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="G148" s="21" t="s">
+      <c r="G148" s="25" t="s">
         <v>359</v>
       </c>
-      <c r="H148" s="22"/>
-      <c r="I148" s="23"/>
-      <c r="J148" s="20"/>
+      <c r="H148" s="24"/>
+      <c r="I148" s="26"/>
+      <c r="J148" s="27"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="20">
+      <c r="A149" s="27">
         <v>147</v>
       </c>
-      <c r="B149" s="20">
+      <c r="B149" s="27">
         <v>6</v>
       </c>
-      <c r="C149" s="21" t="s">
+      <c r="C149" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D149" s="22">
+      <c r="D149" s="24">
         <v>6.7</v>
       </c>
-      <c r="E149" s="21" t="s">
+      <c r="E149" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F149" s="22" t="s">
+      <c r="F149" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="G149" s="21" t="s">
+      <c r="G149" s="25" t="s">
         <v>361</v>
       </c>
-      <c r="H149" s="22"/>
-      <c r="I149" s="23"/>
-      <c r="J149" s="20"/>
+      <c r="H149" s="24"/>
+      <c r="I149" s="26"/>
+      <c r="J149" s="27"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="20">
+      <c r="A150" s="27">
         <v>148</v>
       </c>
-      <c r="B150" s="20">
+      <c r="B150" s="27">
         <v>6</v>
       </c>
-      <c r="C150" s="21" t="s">
+      <c r="C150" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D150" s="22">
+      <c r="D150" s="24">
         <v>6.7</v>
       </c>
-      <c r="E150" s="21" t="s">
+      <c r="E150" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F150" s="22" t="s">
+      <c r="F150" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="G150" s="21" t="s">
+      <c r="G150" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="H150" s="22"/>
-      <c r="I150" s="23"/>
-      <c r="J150" s="20"/>
+      <c r="H150" s="24"/>
+      <c r="I150" s="26"/>
+      <c r="J150" s="27"/>
     </row>
     <row r="151" spans="1:10">
-      <c r="A151" s="20">
+      <c r="A151" s="27">
         <v>149</v>
       </c>
-      <c r="B151" s="20">
+      <c r="B151" s="27">
         <v>6</v>
       </c>
-      <c r="C151" s="21" t="s">
+      <c r="C151" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D151" s="22">
+      <c r="D151" s="24">
         <v>6.8</v>
       </c>
-      <c r="E151" s="21" t="s">
+      <c r="E151" s="25" t="s">
         <v>585</v>
       </c>
-      <c r="F151" s="28" t="s">
+      <c r="F151" s="40" t="s">
         <v>364</v>
       </c>
-      <c r="G151" s="21" t="s">
+      <c r="G151" s="25" t="s">
         <v>365</v>
       </c>
-      <c r="H151" s="22"/>
-      <c r="I151" s="23"/>
-      <c r="J151" s="20"/>
+      <c r="H151" s="24"/>
+      <c r="I151" s="26"/>
+      <c r="J151" s="27"/>
     </row>
     <row r="152" spans="1:10">
-      <c r="A152" s="20">
+      <c r="A152" s="27">
         <v>150</v>
       </c>
-      <c r="B152" s="20">
+      <c r="B152" s="27">
         <v>6</v>
       </c>
-      <c r="C152" s="21" t="s">
+      <c r="C152" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D152" s="22">
+      <c r="D152" s="24">
         <v>6.8</v>
       </c>
-      <c r="E152" s="21" t="s">
+      <c r="E152" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F152" s="22" t="s">
+      <c r="F152" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G152" s="29" t="s">
+      <c r="G152" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="H152" s="22"/>
-      <c r="I152" s="23"/>
-      <c r="J152" s="20">
+      <c r="H152" s="24"/>
+      <c r="I152" s="26"/>
+      <c r="J152" s="27">
         <v>467</v>
       </c>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="20">
+      <c r="A153" s="27">
         <v>151</v>
       </c>
-      <c r="B153" s="20">
+      <c r="B153" s="27">
         <v>7</v>
       </c>
-      <c r="C153" s="21" t="s">
+      <c r="C153" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D153" s="22">
+      <c r="D153" s="24">
         <v>7.1</v>
       </c>
-      <c r="E153" s="21" t="s">
+      <c r="E153" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F153" s="22" t="s">
+      <c r="F153" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="G153" s="21" t="s">
+      <c r="G153" s="25" t="s">
         <v>369</v>
       </c>
-      <c r="H153" s="22"/>
-      <c r="I153" s="23"/>
-      <c r="J153" s="20"/>
+      <c r="H153" s="24"/>
+      <c r="I153" s="26"/>
+      <c r="J153" s="27"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="20">
+      <c r="A154" s="27">
         <v>152</v>
       </c>
-      <c r="B154" s="20">
+      <c r="B154" s="27">
         <v>7</v>
       </c>
-      <c r="C154" s="21" t="s">
+      <c r="C154" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D154" s="22">
+      <c r="D154" s="24">
         <v>7.1</v>
       </c>
-      <c r="E154" s="21" t="s">
+      <c r="E154" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F154" s="22" t="s">
+      <c r="F154" s="24" t="s">
         <v>370</v>
       </c>
-      <c r="G154" s="21" t="s">
+      <c r="G154" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="H154" s="22"/>
-      <c r="I154" s="23"/>
-      <c r="J154" s="20"/>
+      <c r="H154" s="24"/>
+      <c r="I154" s="26"/>
+      <c r="J154" s="27"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="20">
+      <c r="A155" s="27">
         <v>153</v>
       </c>
-      <c r="B155" s="20">
+      <c r="B155" s="27">
         <v>7</v>
       </c>
-      <c r="C155" s="21" t="s">
+      <c r="C155" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D155" s="22">
+      <c r="D155" s="24">
         <v>7.1</v>
       </c>
-      <c r="E155" s="21" t="s">
+      <c r="E155" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F155" s="22" t="s">
+      <c r="F155" s="24" t="s">
         <v>372</v>
       </c>
-      <c r="G155" s="21" t="s">
+      <c r="G155" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="H155" s="22"/>
-      <c r="I155" s="23"/>
-      <c r="J155" s="20"/>
+      <c r="H155" s="24"/>
+      <c r="I155" s="26"/>
+      <c r="J155" s="27"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="20">
+      <c r="A156" s="27">
         <v>154</v>
       </c>
-      <c r="B156" s="20">
+      <c r="B156" s="27">
         <v>7</v>
       </c>
-      <c r="C156" s="21" t="s">
+      <c r="C156" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D156" s="22">
+      <c r="D156" s="24">
         <v>7.1</v>
       </c>
-      <c r="E156" s="21" t="s">
+      <c r="E156" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F156" s="22" t="s">
+      <c r="F156" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="G156" s="21" t="s">
+      <c r="G156" s="25" t="s">
         <v>375</v>
       </c>
-      <c r="H156" s="22"/>
-      <c r="I156" s="23"/>
-      <c r="J156" s="20"/>
+      <c r="H156" s="24"/>
+      <c r="I156" s="26"/>
+      <c r="J156" s="27"/>
     </row>
     <row r="157" spans="1:10">
-      <c r="A157" s="20">
+      <c r="A157" s="27">
         <v>155</v>
       </c>
-      <c r="B157" s="20">
+      <c r="B157" s="27">
         <v>7</v>
       </c>
-      <c r="C157" s="21" t="s">
+      <c r="C157" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D157" s="22">
+      <c r="D157" s="24">
         <v>7.2</v>
       </c>
-      <c r="E157" s="20" t="s">
+      <c r="E157" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F157" s="22" t="s">
+      <c r="F157" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="G157" s="21" t="s">
+      <c r="G157" s="25" t="s">
         <v>377</v>
       </c>
-      <c r="H157" s="22"/>
-      <c r="I157" s="23"/>
-      <c r="J157" s="20"/>
+      <c r="H157" s="24"/>
+      <c r="I157" s="26"/>
+      <c r="J157" s="27"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="20">
+      <c r="A158" s="27">
         <v>156</v>
       </c>
-      <c r="B158" s="20">
+      <c r="B158" s="27">
         <v>7</v>
       </c>
-      <c r="C158" s="21" t="s">
+      <c r="C158" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D158" s="22">
+      <c r="D158" s="24">
         <v>7.3</v>
       </c>
-      <c r="E158" s="21" t="s">
+      <c r="E158" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F158" s="22" t="s">
+      <c r="F158" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="G158" s="21" t="s">
+      <c r="G158" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="H158" s="22"/>
-      <c r="I158" s="23"/>
-      <c r="J158" s="20"/>
+      <c r="H158" s="24"/>
+      <c r="I158" s="26"/>
+      <c r="J158" s="27"/>
     </row>
     <row r="159" spans="1:10">
-      <c r="A159" s="20">
+      <c r="A159" s="27">
         <v>157</v>
       </c>
-      <c r="B159" s="20">
+      <c r="B159" s="27">
         <v>7</v>
       </c>
-      <c r="C159" s="21" t="s">
+      <c r="C159" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D159" s="22">
+      <c r="D159" s="24">
         <v>7.3</v>
       </c>
-      <c r="E159" s="21" t="s">
+      <c r="E159" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F159" s="22" t="s">
+      <c r="F159" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="G159" s="21" t="s">
+      <c r="G159" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="H159" s="22"/>
-      <c r="I159" s="23"/>
-      <c r="J159" s="20"/>
+      <c r="H159" s="24"/>
+      <c r="I159" s="26"/>
+      <c r="J159" s="27"/>
     </row>
     <row r="160" spans="1:10">
-      <c r="A160" s="20">
+      <c r="A160" s="27">
         <v>158</v>
       </c>
-      <c r="B160" s="20">
+      <c r="B160" s="27">
         <v>7</v>
       </c>
-      <c r="C160" s="21" t="s">
+      <c r="C160" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D160" s="22">
+      <c r="D160" s="24">
         <v>7.3</v>
       </c>
-      <c r="E160" s="21" t="s">
+      <c r="E160" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F160" s="22" t="s">
+      <c r="F160" s="24" t="s">
         <v>381</v>
       </c>
-      <c r="G160" s="21" t="s">
+      <c r="G160" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="H160" s="22"/>
-      <c r="I160" s="23"/>
-      <c r="J160" s="20"/>
+      <c r="H160" s="24"/>
+      <c r="I160" s="26"/>
+      <c r="J160" s="27"/>
     </row>
     <row r="161" spans="1:10">
-      <c r="A161" s="20">
+      <c r="A161" s="27">
         <v>159</v>
       </c>
-      <c r="B161" s="20">
+      <c r="B161" s="27">
         <v>7</v>
       </c>
-      <c r="C161" s="21" t="s">
+      <c r="C161" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D161" s="22">
+      <c r="D161" s="24">
         <v>7.3</v>
       </c>
-      <c r="E161" s="21" t="s">
+      <c r="E161" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F161" s="22" t="s">
+      <c r="F161" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="G161" s="21" t="s">
+      <c r="G161" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="H161" s="22"/>
-      <c r="I161" s="23"/>
-      <c r="J161" s="20">
+      <c r="H161" s="24"/>
+      <c r="I161" s="26"/>
+      <c r="J161" s="27">
         <v>502</v>
       </c>
     </row>
@@ -19345,7 +19721,7 @@
       <c r="F195" s="22" t="s">
         <v>451</v>
       </c>
-      <c r="G195" s="31" t="s">
+      <c r="G195" s="29" t="s">
         <v>452</v>
       </c>
       <c r="H195" s="22"/>
@@ -19371,7 +19747,7 @@
       <c r="F196" s="22" t="s">
         <v>453</v>
       </c>
-      <c r="G196" s="31" t="s">
+      <c r="G196" s="29" t="s">
         <v>454</v>
       </c>
       <c r="H196" s="22"/>
@@ -19397,7 +19773,7 @@
       <c r="F197" s="22" t="s">
         <v>455</v>
       </c>
-      <c r="G197" s="31" t="s">
+      <c r="G197" s="29" t="s">
         <v>456</v>
       </c>
       <c r="H197" s="22"/>
@@ -19987,15 +20363,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>530</v>
       </c>
@@ -20006,7 +20382,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20017,7 +20393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -20028,7 +20404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -20039,7 +20415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -20050,7 +20426,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -20061,7 +20437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -20072,7 +20448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -20083,7 +20459,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20094,7 +20470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20105,7 +20481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>529</v>
       </c>
@@ -20118,6 +20494,76 @@
         <v>217</v>
       </c>
       <c r="D11" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="F13" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>601</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="H14" s="32"/>
+      <c r="I14" s="30" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>602</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>616</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>613</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>611</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="30" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>614</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>612</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="34"/>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="G17" s="36"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="39" t="s">
+        <v>617</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>